<commit_message>
Lista Maestra de requerimientos
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/LMREQM/LMREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/LMREQM/LMREQM_V1.1_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\LMREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_REQM\LMREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" tabRatio="767" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" tabRatio="767" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="34" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="TipoProyecto">'Diccionario de atributos-valor'!$E$20:$E$23</definedName>
     <definedName name="TipoRequerimientoDeSistema">'Diccionario de atributos-valor'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -247,9 +247,6 @@
     <t>Aprobado</t>
   </si>
   <si>
-    <t>Versión: 1.0</t>
-  </si>
-  <si>
     <t>Representa el nombre de la persona que puede proveer información sobre el requerimiento.</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
     <t>Desarrollo</t>
   </si>
   <si>
-    <t>Fecha Efectiva: 13/10/2015</t>
-  </si>
-  <si>
     <t>Roger Apaestegui (Jefe de Proyecto)</t>
   </si>
   <si>
@@ -389,9 +383,6 @@
   </si>
   <si>
     <t>Jefe de Proyecto</t>
-  </si>
-  <si>
-    <t>Version Preliminar</t>
   </si>
   <si>
     <r>
@@ -596,12 +587,6 @@
     <t>Julio Leonardo Paredes</t>
   </si>
   <si>
-    <t>Version Preliminar Aprobada por QA</t>
-  </si>
-  <si>
-    <t>En Revisión</t>
-  </si>
-  <si>
     <t xml:space="preserve">Analista de Calidad </t>
   </si>
   <si>
@@ -705,11 +690,26 @@
   <si>
     <t>Manuel Sáenz Tarazona (MST E.I.R.L.)</t>
   </si>
+  <si>
+    <t>Version Preliminar Revisada por QA</t>
+  </si>
+  <si>
+    <t>Revisado</t>
+  </si>
+  <si>
+    <t>Version Final pendiente de Aprobación</t>
+  </si>
+  <si>
+    <t>Fecha Efectiva: 19/11/2015</t>
+  </si>
+  <si>
+    <t>Versión: 1.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1352,7 +1352,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1541,9 +1541,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1733,6 +1730,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1745,173 +1745,170 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1924,6 +1921,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1958,6 +1959,60 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1979,66 +2034,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2795,7 +2798,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2822,15 +2825,15 @@
     </row>
     <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="55"/>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
       <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9">
@@ -2875,22 +2878,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D5" s="138">
         <v>42290</v>
       </c>
       <c r="E5" s="136" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F5" s="136" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="G5" s="136" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="H5" s="136" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I5" s="55"/>
     </row>
@@ -2910,22 +2913,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="137" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="138">
+        <v>42327</v>
+      </c>
+      <c r="E7" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="136" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="136" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="136" t="s">
         <v>152</v>
-      </c>
-      <c r="D7" s="138">
-        <v>42313</v>
-      </c>
-      <c r="E7" s="136" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="136" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="136" t="s">
-        <v>157</v>
-      </c>
-      <c r="H7" s="136" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2939,6 +2942,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2947,13 +2957,6 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2967,7 +2970,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2996,93 +2999,93 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="74"/>
-      <c r="E2" s="184" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
+      <c r="E2" s="158" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="185" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-    </row>
-    <row r="4" spans="1:8" s="80" customFormat="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-    </row>
-    <row r="5" spans="1:8" s="80" customFormat="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76" t="s">
+      <c r="D3" s="235" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="234" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+    </row>
+    <row r="4" spans="1:8" s="79" customFormat="1">
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+    </row>
+    <row r="5" spans="1:8" s="79" customFormat="1">
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="191" t="s">
+      <c r="D6" s="165" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="191"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="191"/>
-      <c r="H6" s="191"/>
-    </row>
-    <row r="7" spans="1:8" s="80" customFormat="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-    </row>
-    <row r="8" spans="1:8" s="80" customFormat="1">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+    </row>
+    <row r="7" spans="1:8" s="79" customFormat="1">
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+    </row>
+    <row r="8" spans="1:8" s="79" customFormat="1">
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="186" t="s">
+      <c r="D9" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="187"/>
+      <c r="E9" s="161"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="192"/>
+      <c r="H9" s="166"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9"/>
@@ -3096,14 +3099,14 @@
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="188" t="s">
+      <c r="D11" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="188"/>
-      <c r="G11" s="193" t="s">
+      <c r="E11" s="162"/>
+      <c r="G11" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="193"/>
+      <c r="H11" s="167"/>
     </row>
     <row r="12" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="9"/>
@@ -3116,14 +3119,14 @@
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="189" t="s">
+      <c r="D13" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="189"/>
-      <c r="G13" s="193" t="s">
+      <c r="E13" s="163"/>
+      <c r="G13" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="193"/>
+      <c r="H13" s="167"/>
     </row>
     <row r="14" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A14" s="9"/>
@@ -3134,14 +3137,14 @@
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="190" t="s">
+      <c r="D15" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="190"/>
-      <c r="G15" s="193" t="s">
+      <c r="E15" s="164"/>
+      <c r="G15" s="167" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="193"/>
+      <c r="H15" s="167"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="7"/>
@@ -3152,14 +3155,14 @@
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="183" t="s">
+      <c r="D17" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="183"/>
-      <c r="G17" s="193" t="s">
+      <c r="E17" s="155"/>
+      <c r="G17" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="193"/>
+      <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:8" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="15"/>
@@ -3176,79 +3179,79 @@
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:8" s="19" customFormat="1" ht="16.5" customHeight="1">
-      <c r="D20" s="150" t="s">
+      <c r="D20" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="153"/>
     </row>
     <row r="21" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D21" s="181" t="s">
+      <c r="D21" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="151" t="s">
+      <c r="E21" s="142"/>
+      <c r="F21" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="151"/>
-      <c r="H21" s="151"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="154"/>
     </row>
     <row r="22" spans="1:8" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="D22" s="179" t="s">
+      <c r="D22" s="156" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="180"/>
-      <c r="F22" s="149" t="s">
+      <c r="E22" s="157"/>
+      <c r="F22" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="149"/>
-      <c r="H22" s="149"/>
+      <c r="G22" s="168"/>
+      <c r="H22" s="168"/>
     </row>
     <row r="23" spans="1:8" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="D23" s="179" t="s">
+      <c r="D23" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="180"/>
-      <c r="F23" s="149" t="s">
+      <c r="E23" s="157"/>
+      <c r="F23" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="149"/>
-      <c r="H23" s="149"/>
+      <c r="G23" s="168"/>
+      <c r="H23" s="168"/>
     </row>
     <row r="24" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D24" s="179" t="s">
+      <c r="D24" s="156" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="157"/>
+      <c r="F24" s="172" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="173"/>
+      <c r="H24" s="174"/>
+    </row>
+    <row r="25" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
+      <c r="D25" s="156" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="157"/>
+      <c r="F25" s="168" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="180"/>
-      <c r="F24" s="168" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="169"/>
-      <c r="H24" s="170"/>
-    </row>
-    <row r="25" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D25" s="179" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="180"/>
-      <c r="F25" s="149" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="149"/>
-      <c r="H25" s="149"/>
+      <c r="G25" s="168"/>
+      <c r="H25" s="168"/>
     </row>
     <row r="26" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D26" s="179" t="s">
+      <c r="D26" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="180"/>
-      <c r="F26" s="149" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="149"/>
-      <c r="H26" s="149"/>
+      <c r="E26" s="157"/>
+      <c r="F26" s="168" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="168"/>
+      <c r="H26" s="168"/>
     </row>
     <row r="27" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
       <c r="D27" s="50"/>
@@ -3265,183 +3268,183 @@
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:8" s="19" customFormat="1" ht="16.5" customHeight="1">
-      <c r="D29" s="150" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
-      <c r="G29" s="150"/>
-      <c r="H29" s="150"/>
+      <c r="D29" s="153" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="153"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="153"/>
     </row>
     <row r="30" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D30" s="181" t="s">
+      <c r="D30" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="182"/>
-      <c r="F30" s="151" t="s">
+      <c r="E30" s="142"/>
+      <c r="F30" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="154"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="152" t="s">
+      <c r="D31" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="152"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="153"/>
-      <c r="H31" s="153"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="149"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="173" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="174"/>
-      <c r="F32" s="154" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="155"/>
-      <c r="H32" s="156"/>
+      <c r="D32" s="179" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="180"/>
+      <c r="F32" s="150" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="151"/>
+      <c r="H32" s="152"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="173" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="174"/>
-      <c r="F33" s="154" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="155"/>
-      <c r="H33" s="156"/>
+      <c r="D33" s="179" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="180"/>
+      <c r="F33" s="150" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="151"/>
+      <c r="H33" s="152"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="157" t="s">
+      <c r="D34" s="183" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="157"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="158"/>
-      <c r="H34" s="158"/>
+      <c r="E34" s="183"/>
+      <c r="F34" s="184"/>
+      <c r="G34" s="184"/>
+      <c r="H34" s="184"/>
     </row>
     <row r="35" spans="1:8" ht="24.75" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="173" t="s">
+      <c r="D35" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="174"/>
-      <c r="F35" s="159" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="160"/>
-      <c r="H35" s="161"/>
+      <c r="E35" s="180"/>
+      <c r="F35" s="169" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="170"/>
+      <c r="H35" s="171"/>
     </row>
     <row r="36" spans="1:8" ht="24.75" customHeight="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="173" t="s">
+      <c r="D36" s="179" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="174"/>
-      <c r="F36" s="159" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36" s="160"/>
-      <c r="H36" s="161"/>
+      <c r="E36" s="180"/>
+      <c r="F36" s="169" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="170"/>
+      <c r="H36" s="171"/>
     </row>
     <row r="37" spans="1:8" ht="42" customHeight="1">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="173" t="s">
+      <c r="D37" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="174"/>
-      <c r="F37" s="159" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="160"/>
-      <c r="H37" s="161"/>
+      <c r="E37" s="180"/>
+      <c r="F37" s="169" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="170"/>
+      <c r="H37" s="171"/>
     </row>
     <row r="38" spans="1:8" ht="354" customHeight="1">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="166" t="s">
+      <c r="D38" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="167"/>
-      <c r="F38" s="164" t="s">
-        <v>109</v>
-      </c>
-      <c r="G38" s="171"/>
-      <c r="H38" s="171"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="176" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="177"/>
+      <c r="H38" s="177"/>
     </row>
     <row r="39" spans="1:8" s="19" customFormat="1" ht="25.5" customHeight="1">
-      <c r="D39" s="175" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" s="176"/>
-      <c r="F39" s="172" t="s">
+      <c r="D39" s="145" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="146"/>
+      <c r="F39" s="178" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="171"/>
-      <c r="H39" s="171"/>
+      <c r="G39" s="177"/>
+      <c r="H39" s="177"/>
     </row>
     <row r="40" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D40" s="175" t="s">
+      <c r="D40" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="146"/>
+      <c r="F40" s="176" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+    </row>
+    <row r="41" spans="1:8" s="19" customFormat="1" ht="24" customHeight="1">
+      <c r="D41" s="181" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="176"/>
-      <c r="F40" s="164" t="s">
-        <v>77</v>
-      </c>
-      <c r="G40" s="165"/>
-      <c r="H40" s="165"/>
-    </row>
-    <row r="41" spans="1:8" s="19" customFormat="1" ht="24" customHeight="1">
-      <c r="D41" s="177" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="178"/>
-      <c r="F41" s="191" t="s">
-        <v>166</v>
-      </c>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
+      <c r="E41" s="182"/>
+      <c r="F41" s="165" t="s">
+        <v>161</v>
+      </c>
+      <c r="G41" s="185"/>
+      <c r="H41" s="185"/>
     </row>
     <row r="42" spans="1:8" s="19" customFormat="1" ht="25.5" customHeight="1">
-      <c r="D42" s="177" t="s">
+      <c r="D42" s="181" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="182"/>
+      <c r="F42" s="176" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="178"/>
-      <c r="F42" s="164" t="s">
-        <v>74</v>
-      </c>
-      <c r="G42" s="165"/>
-      <c r="H42" s="165"/>
+      <c r="G42" s="185"/>
+      <c r="H42" s="185"/>
     </row>
     <row r="43" spans="1:8" s="19" customFormat="1">
       <c r="D43" s="51"/>
       <c r="E43" s="51"/>
       <c r="F43" s="51"/>
-      <c r="G43" s="83"/>
-      <c r="H43" s="83"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="82"/>
     </row>
     <row r="44" spans="1:8" ht="13.5">
       <c r="A44" s="7"/>
@@ -3454,125 +3457,125 @@
       <c r="H44" s="73"/>
     </row>
     <row r="45" spans="1:8" s="19" customFormat="1" ht="16.5" customHeight="1">
-      <c r="D45" s="150" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" s="150"/>
-      <c r="F45" s="150"/>
-      <c r="G45" s="150"/>
-      <c r="H45" s="150"/>
+      <c r="D45" s="153" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="153"/>
+      <c r="F45" s="153"/>
+      <c r="G45" s="153"/>
+      <c r="H45" s="153"/>
     </row>
     <row r="46" spans="1:8" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D46" s="181" t="s">
+      <c r="D46" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="182"/>
-      <c r="F46" s="151" t="s">
+      <c r="E46" s="142"/>
+      <c r="F46" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="G46" s="151"/>
-      <c r="H46" s="151"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="154"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="152" t="s">
+      <c r="D47" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="152"/>
-      <c r="F47" s="153"/>
-      <c r="G47" s="153"/>
-      <c r="H47" s="153"/>
+      <c r="E47" s="148"/>
+      <c r="F47" s="149"/>
+      <c r="G47" s="149"/>
+      <c r="H47" s="149"/>
     </row>
     <row r="48" spans="1:8" s="68" customFormat="1">
       <c r="A48" s="67"/>
       <c r="B48" s="67"/>
       <c r="C48" s="67"/>
-      <c r="D48" s="194" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" s="167"/>
-      <c r="F48" s="154" t="s">
-        <v>159</v>
-      </c>
-      <c r="G48" s="155"/>
-      <c r="H48" s="156"/>
+      <c r="D48" s="143" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="144"/>
+      <c r="F48" s="150" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48" s="151"/>
+      <c r="H48" s="152"/>
     </row>
     <row r="49" spans="1:255" s="68" customFormat="1" ht="12" customHeight="1">
       <c r="A49" s="67"/>
       <c r="B49" s="67"/>
       <c r="C49" s="67"/>
-      <c r="D49" s="175" t="s">
+      <c r="D49" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="176"/>
-      <c r="F49" s="154" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="155"/>
-      <c r="H49" s="156"/>
+      <c r="E49" s="146"/>
+      <c r="F49" s="150" t="s">
+        <v>62</v>
+      </c>
+      <c r="G49" s="151"/>
+      <c r="H49" s="152"/>
     </row>
     <row r="50" spans="1:255" s="68" customFormat="1">
       <c r="A50" s="67"/>
       <c r="B50" s="67"/>
       <c r="C50" s="67"/>
-      <c r="D50" s="152" t="s">
+      <c r="D50" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="152"/>
-      <c r="F50" s="153"/>
-      <c r="G50" s="153"/>
-      <c r="H50" s="153"/>
+      <c r="E50" s="148"/>
+      <c r="F50" s="149"/>
+      <c r="G50" s="149"/>
+      <c r="H50" s="149"/>
     </row>
     <row r="51" spans="1:255" s="68" customFormat="1">
       <c r="A51" s="67"/>
       <c r="B51" s="67"/>
       <c r="C51" s="67"/>
-      <c r="D51" s="166" t="s">
+      <c r="D51" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="167"/>
-      <c r="F51" s="154" t="s">
-        <v>94</v>
-      </c>
-      <c r="G51" s="155"/>
-      <c r="H51" s="156"/>
+      <c r="E51" s="144"/>
+      <c r="F51" s="150" t="s">
+        <v>93</v>
+      </c>
+      <c r="G51" s="151"/>
+      <c r="H51" s="152"/>
     </row>
     <row r="52" spans="1:255" s="68" customFormat="1">
       <c r="A52" s="67"/>
       <c r="B52" s="67"/>
       <c r="C52" s="67"/>
-      <c r="D52" s="166" t="s">
+      <c r="D52" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="167"/>
-      <c r="F52" s="154" t="s">
-        <v>167</v>
-      </c>
-      <c r="G52" s="155"/>
-      <c r="H52" s="156"/>
+      <c r="E52" s="144"/>
+      <c r="F52" s="150" t="s">
+        <v>162</v>
+      </c>
+      <c r="G52" s="151"/>
+      <c r="H52" s="152"/>
     </row>
     <row r="53" spans="1:255" s="68" customFormat="1">
       <c r="A53" s="67"/>
       <c r="B53" s="67"/>
       <c r="C53" s="67"/>
-      <c r="D53" s="166" t="s">
+      <c r="D53" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="E53" s="167"/>
-      <c r="F53" s="154" t="s">
+      <c r="E53" s="144"/>
+      <c r="F53" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="G53" s="155"/>
-      <c r="H53" s="156"/>
+      <c r="G53" s="151"/>
+      <c r="H53" s="152"/>
     </row>
     <row r="54" spans="1:255" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
     </row>
     <row r="55" spans="1:255" ht="13.5">
       <c r="A55" s="7"/>
@@ -3585,64 +3588,64 @@
       <c r="H55" s="73"/>
     </row>
     <row r="56" spans="1:255" s="19" customFormat="1" ht="16.5" customHeight="1">
-      <c r="D56" s="150" t="s">
+      <c r="D56" s="153" t="s">
         <v>44</v>
       </c>
-      <c r="E56" s="150"/>
-      <c r="F56" s="150"/>
-      <c r="G56" s="150"/>
-      <c r="H56" s="150"/>
+      <c r="E56" s="153"/>
+      <c r="F56" s="153"/>
+      <c r="G56" s="153"/>
+      <c r="H56" s="153"/>
     </row>
     <row r="57" spans="1:255" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D57" s="181" t="s">
+      <c r="D57" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="182"/>
-      <c r="F57" s="151" t="s">
+      <c r="E57" s="142"/>
+      <c r="F57" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="G57" s="151"/>
-      <c r="H57" s="151"/>
+      <c r="G57" s="154"/>
+      <c r="H57" s="154"/>
     </row>
     <row r="58" spans="1:255">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
-      <c r="D58" s="152" t="s">
+      <c r="D58" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="E58" s="152"/>
-      <c r="F58" s="153"/>
-      <c r="G58" s="153"/>
-      <c r="H58" s="153"/>
+      <c r="E58" s="148"/>
+      <c r="F58" s="149"/>
+      <c r="G58" s="149"/>
+      <c r="H58" s="149"/>
     </row>
     <row r="59" spans="1:255" s="69" customFormat="1">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
-      <c r="D59" s="166" t="s">
+      <c r="D59" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="167"/>
-      <c r="F59" s="154" t="s">
-        <v>168</v>
-      </c>
-      <c r="G59" s="155"/>
-      <c r="H59" s="156"/>
+      <c r="E59" s="144"/>
+      <c r="F59" s="150" t="s">
+        <v>163</v>
+      </c>
+      <c r="G59" s="151"/>
+      <c r="H59" s="152"/>
     </row>
     <row r="60" spans="1:255" s="69" customFormat="1">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
-      <c r="D60" s="166" t="s">
+      <c r="D60" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="167"/>
-      <c r="F60" s="154" t="s">
-        <v>169</v>
-      </c>
-      <c r="G60" s="155"/>
-      <c r="H60" s="156"/>
+      <c r="E60" s="144"/>
+      <c r="F60" s="150" t="s">
+        <v>164</v>
+      </c>
+      <c r="G60" s="151"/>
+      <c r="H60" s="152"/>
     </row>
     <row r="61" spans="1:255" ht="18" customHeight="1">
       <c r="A61" s="7"/>
@@ -3651,17 +3654,17 @@
       <c r="D61" s="51"/>
       <c r="E61" s="51"/>
       <c r="F61" s="52"/>
-      <c r="G61" s="83"/>
-      <c r="H61" s="83"/>
+      <c r="G61" s="82"/>
+      <c r="H61" s="82"/>
     </row>
     <row r="62" spans="1:255" s="19" customFormat="1" ht="13.5" customHeight="1">
-      <c r="D62" s="150" t="s">
+      <c r="D62" s="153" t="s">
         <v>44</v>
       </c>
-      <c r="E62" s="150"/>
-      <c r="F62" s="150"/>
-      <c r="G62" s="150"/>
-      <c r="H62" s="150"/>
+      <c r="E62" s="153"/>
+      <c r="F62" s="153"/>
+      <c r="G62" s="153"/>
+      <c r="H62" s="153"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
@@ -3913,83 +3916,83 @@
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="181" t="s">
+      <c r="D63" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E63" s="182"/>
-      <c r="F63" s="151" t="s">
+      <c r="E63" s="142"/>
+      <c r="F63" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="G63" s="151"/>
-      <c r="H63" s="151"/>
+      <c r="G63" s="154"/>
+      <c r="H63" s="154"/>
     </row>
     <row r="64" spans="1:255">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="152" t="s">
+      <c r="D64" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="E64" s="152"/>
-      <c r="F64" s="153"/>
-      <c r="G64" s="153"/>
-      <c r="H64" s="153"/>
+      <c r="E64" s="148"/>
+      <c r="F64" s="149"/>
+      <c r="G64" s="149"/>
+      <c r="H64" s="149"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
-      <c r="D65" s="162" t="s">
+      <c r="D65" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="E65" s="163"/>
-      <c r="F65" s="154" t="s">
-        <v>95</v>
-      </c>
-      <c r="G65" s="155"/>
-      <c r="H65" s="156"/>
+      <c r="E65" s="140"/>
+      <c r="F65" s="150" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="151"/>
+      <c r="H65" s="152"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
-      <c r="D66" s="162" t="s">
+      <c r="D66" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="E66" s="163"/>
-      <c r="F66" s="154" t="s">
-        <v>96</v>
-      </c>
-      <c r="G66" s="155"/>
-      <c r="H66" s="156"/>
+      <c r="E66" s="140"/>
+      <c r="F66" s="150" t="s">
+        <v>95</v>
+      </c>
+      <c r="G66" s="151"/>
+      <c r="H66" s="152"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="162" t="s">
+      <c r="D67" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="E67" s="163"/>
-      <c r="F67" s="154" t="s">
-        <v>97</v>
-      </c>
-      <c r="G67" s="155"/>
-      <c r="H67" s="156"/>
+      <c r="E67" s="140"/>
+      <c r="F67" s="150" t="s">
+        <v>96</v>
+      </c>
+      <c r="G67" s="151"/>
+      <c r="H67" s="152"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
-      <c r="D68" s="162" t="s">
+      <c r="D68" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="E68" s="163"/>
-      <c r="F68" s="154" t="s">
-        <v>98</v>
-      </c>
-      <c r="G68" s="155"/>
-      <c r="H68" s="156"/>
+      <c r="E68" s="140"/>
+      <c r="F68" s="150" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="151"/>
+      <c r="H68" s="152"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="15"/>
@@ -4035,9 +4038,9 @@
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
-      <c r="D73" s="147"/>
-      <c r="E73" s="147"/>
-      <c r="F73" s="147"/>
+      <c r="D73" s="175"/>
+      <c r="E73" s="175"/>
+      <c r="F73" s="175"/>
       <c r="G73" s="17"/>
       <c r="H73" s="17"/>
     </row>
@@ -4065,9 +4068,9 @@
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
-      <c r="D76" s="147"/>
-      <c r="E76" s="147"/>
-      <c r="F76" s="147"/>
+      <c r="D76" s="175"/>
+      <c r="E76" s="175"/>
+      <c r="F76" s="175"/>
       <c r="G76" s="23"/>
       <c r="H76" s="17"/>
     </row>
@@ -4115,9 +4118,9 @@
       <c r="A81" s="15"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
-      <c r="D81" s="147"/>
-      <c r="E81" s="147"/>
-      <c r="F81" s="147"/>
+      <c r="D81" s="175"/>
+      <c r="E81" s="175"/>
+      <c r="F81" s="175"/>
       <c r="G81" s="23"/>
       <c r="H81" s="17"/>
     </row>
@@ -4182,9 +4185,9 @@
       <c r="A88" s="15"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
-      <c r="D88" s="147"/>
-      <c r="E88" s="147"/>
-      <c r="F88" s="147"/>
+      <c r="D88" s="175"/>
+      <c r="E88" s="175"/>
+      <c r="F88" s="175"/>
       <c r="G88" s="17"/>
       <c r="H88" s="17"/>
     </row>
@@ -4192,9 +4195,9 @@
       <c r="A89" s="15"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
-      <c r="D89" s="147"/>
-      <c r="E89" s="147"/>
-      <c r="F89" s="147"/>
+      <c r="D89" s="175"/>
+      <c r="E89" s="175"/>
+      <c r="F89" s="175"/>
       <c r="G89" s="17"/>
       <c r="H89" s="17"/>
     </row>
@@ -4202,9 +4205,9 @@
       <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
-      <c r="D90" s="147"/>
-      <c r="E90" s="147"/>
-      <c r="F90" s="147"/>
+      <c r="D90" s="175"/>
+      <c r="E90" s="175"/>
+      <c r="F90" s="175"/>
       <c r="G90" s="17"/>
       <c r="H90" s="17"/>
     </row>
@@ -4212,9 +4215,9 @@
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
-      <c r="D91" s="147"/>
-      <c r="E91" s="147"/>
-      <c r="F91" s="147"/>
+      <c r="D91" s="175"/>
+      <c r="E91" s="175"/>
+      <c r="F91" s="175"/>
       <c r="G91" s="23"/>
       <c r="H91" s="17"/>
     </row>
@@ -4463,8 +4466,8 @@
       <c r="D116" s="32"/>
       <c r="E116" s="32"/>
       <c r="F116" s="17"/>
-      <c r="G116" s="146"/>
-      <c r="H116" s="146"/>
+      <c r="G116" s="186"/>
+      <c r="H116" s="186"/>
     </row>
     <row r="117" spans="1:8" ht="18.75" customHeight="1">
       <c r="A117" s="15"/>
@@ -4750,11 +4753,11 @@
       <c r="A145" s="17"/>
       <c r="B145" s="17"/>
       <c r="C145" s="17"/>
-      <c r="D145" s="148"/>
-      <c r="E145" s="148"/>
-      <c r="F145" s="148"/>
-      <c r="G145" s="148"/>
-      <c r="H145" s="148"/>
+      <c r="D145" s="187"/>
+      <c r="E145" s="187"/>
+      <c r="F145" s="187"/>
+      <c r="G145" s="187"/>
+      <c r="H145" s="187"/>
     </row>
     <row r="146" spans="1:8">
       <c r="A146" s="17"/>
@@ -4772,9 +4775,9 @@
       <c r="C147" s="17"/>
       <c r="D147" s="42"/>
       <c r="E147" s="42"/>
-      <c r="F147" s="142"/>
-      <c r="G147" s="142"/>
-      <c r="H147" s="142"/>
+      <c r="F147" s="188"/>
+      <c r="G147" s="188"/>
+      <c r="H147" s="188"/>
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="17"/>
@@ -4792,9 +4795,9 @@
       <c r="C149" s="17"/>
       <c r="D149" s="44"/>
       <c r="E149" s="44"/>
-      <c r="F149" s="144"/>
-      <c r="G149" s="142"/>
-      <c r="H149" s="142"/>
+      <c r="F149" s="189"/>
+      <c r="G149" s="188"/>
+      <c r="H149" s="188"/>
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="17"/>
@@ -4812,9 +4815,9 @@
       <c r="C151" s="17"/>
       <c r="D151" s="42"/>
       <c r="E151" s="42"/>
-      <c r="F151" s="142"/>
-      <c r="G151" s="142"/>
-      <c r="H151" s="142"/>
+      <c r="F151" s="188"/>
+      <c r="G151" s="188"/>
+      <c r="H151" s="188"/>
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="17"/>
@@ -4832,9 +4835,9 @@
       <c r="C153" s="17"/>
       <c r="D153" s="44"/>
       <c r="E153" s="44"/>
-      <c r="F153" s="144"/>
-      <c r="G153" s="142"/>
-      <c r="H153" s="142"/>
+      <c r="F153" s="189"/>
+      <c r="G153" s="188"/>
+      <c r="H153" s="188"/>
     </row>
     <row r="154" spans="1:8">
       <c r="A154" s="17"/>
@@ -4862,9 +4865,9 @@
       <c r="C156" s="17"/>
       <c r="D156" s="42"/>
       <c r="E156" s="42"/>
-      <c r="F156" s="142"/>
-      <c r="G156" s="142"/>
-      <c r="H156" s="142"/>
+      <c r="F156" s="188"/>
+      <c r="G156" s="188"/>
+      <c r="H156" s="188"/>
     </row>
     <row r="157" spans="1:8">
       <c r="A157" s="17"/>
@@ -4882,9 +4885,9 @@
       <c r="C158" s="17"/>
       <c r="D158" s="44"/>
       <c r="E158" s="44"/>
-      <c r="F158" s="144"/>
-      <c r="G158" s="142"/>
-      <c r="H158" s="142"/>
+      <c r="F158" s="189"/>
+      <c r="G158" s="188"/>
+      <c r="H158" s="188"/>
     </row>
     <row r="159" spans="1:8" ht="90" customHeight="1">
       <c r="A159" s="17"/>
@@ -4892,9 +4895,9 @@
       <c r="C159" s="17"/>
       <c r="D159" s="44"/>
       <c r="E159" s="44"/>
-      <c r="F159" s="144"/>
-      <c r="G159" s="142"/>
-      <c r="H159" s="142"/>
+      <c r="F159" s="189"/>
+      <c r="G159" s="188"/>
+      <c r="H159" s="188"/>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="17"/>
@@ -4902,9 +4905,9 @@
       <c r="C160" s="17"/>
       <c r="D160" s="44"/>
       <c r="E160" s="44"/>
-      <c r="F160" s="145"/>
-      <c r="G160" s="146"/>
-      <c r="H160" s="146"/>
+      <c r="F160" s="190"/>
+      <c r="G160" s="186"/>
+      <c r="H160" s="186"/>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="17"/>
@@ -4912,8 +4915,8 @@
       <c r="C161" s="17"/>
       <c r="D161" s="46"/>
       <c r="E161" s="46"/>
-      <c r="F161" s="140"/>
-      <c r="G161" s="140"/>
+      <c r="F161" s="191"/>
+      <c r="G161" s="191"/>
       <c r="H161" s="34"/>
     </row>
     <row r="162" spans="1:8">
@@ -4922,8 +4925,8 @@
       <c r="C162" s="17"/>
       <c r="D162" s="46"/>
       <c r="E162" s="46"/>
-      <c r="F162" s="140"/>
-      <c r="G162" s="140"/>
+      <c r="F162" s="191"/>
+      <c r="G162" s="191"/>
       <c r="H162" s="34"/>
     </row>
     <row r="163" spans="1:8">
@@ -4932,8 +4935,8 @@
       <c r="C163" s="17"/>
       <c r="D163" s="46"/>
       <c r="E163" s="46"/>
-      <c r="F163" s="140"/>
-      <c r="G163" s="140"/>
+      <c r="F163" s="191"/>
+      <c r="G163" s="191"/>
       <c r="H163" s="34"/>
     </row>
     <row r="164" spans="1:8">
@@ -4942,8 +4945,8 @@
       <c r="C164" s="17"/>
       <c r="D164" s="46"/>
       <c r="E164" s="46"/>
-      <c r="F164" s="140"/>
-      <c r="G164" s="140"/>
+      <c r="F164" s="191"/>
+      <c r="G164" s="191"/>
       <c r="H164" s="34"/>
     </row>
     <row r="165" spans="1:8">
@@ -4952,8 +4955,8 @@
       <c r="C165" s="17"/>
       <c r="D165" s="46"/>
       <c r="E165" s="46"/>
-      <c r="F165" s="140"/>
-      <c r="G165" s="140"/>
+      <c r="F165" s="191"/>
+      <c r="G165" s="191"/>
       <c r="H165" s="34"/>
     </row>
     <row r="166" spans="1:8">
@@ -4962,8 +4965,8 @@
       <c r="C166" s="17"/>
       <c r="D166" s="46"/>
       <c r="E166" s="46"/>
-      <c r="F166" s="140"/>
-      <c r="G166" s="140"/>
+      <c r="F166" s="191"/>
+      <c r="G166" s="191"/>
       <c r="H166" s="34"/>
     </row>
     <row r="167" spans="1:8">
@@ -4972,8 +4975,8 @@
       <c r="C167" s="17"/>
       <c r="D167" s="46"/>
       <c r="E167" s="46"/>
-      <c r="F167" s="140"/>
-      <c r="G167" s="140"/>
+      <c r="F167" s="191"/>
+      <c r="G167" s="191"/>
       <c r="H167" s="48"/>
     </row>
     <row r="168" spans="1:8">
@@ -4982,8 +4985,8 @@
       <c r="C168" s="17"/>
       <c r="D168" s="46"/>
       <c r="E168" s="46"/>
-      <c r="F168" s="140"/>
-      <c r="G168" s="140"/>
+      <c r="F168" s="191"/>
+      <c r="G168" s="191"/>
       <c r="H168" s="48"/>
     </row>
     <row r="169" spans="1:8">
@@ -4992,8 +4995,8 @@
       <c r="C169" s="17"/>
       <c r="D169" s="46"/>
       <c r="E169" s="46"/>
-      <c r="F169" s="140"/>
-      <c r="G169" s="140"/>
+      <c r="F169" s="191"/>
+      <c r="G169" s="191"/>
       <c r="H169" s="48"/>
     </row>
     <row r="170" spans="1:8">
@@ -5002,8 +5005,8 @@
       <c r="C170" s="17"/>
       <c r="D170" s="46"/>
       <c r="E170" s="46"/>
-      <c r="F170" s="140"/>
-      <c r="G170" s="140"/>
+      <c r="F170" s="191"/>
+      <c r="G170" s="191"/>
       <c r="H170" s="48"/>
     </row>
     <row r="171" spans="1:8" ht="26.25" customHeight="1">
@@ -5012,9 +5015,9 @@
       <c r="C171" s="17"/>
       <c r="D171" s="46"/>
       <c r="E171" s="46"/>
-      <c r="F171" s="143"/>
-      <c r="G171" s="143"/>
-      <c r="H171" s="143"/>
+      <c r="F171" s="192"/>
+      <c r="G171" s="192"/>
+      <c r="H171" s="192"/>
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="17"/>
@@ -5080,9 +5083,9 @@
       <c r="A178" s="17"/>
       <c r="B178" s="17"/>
       <c r="C178" s="17"/>
-      <c r="D178" s="140"/>
-      <c r="E178" s="140"/>
-      <c r="F178" s="140"/>
+      <c r="D178" s="191"/>
+      <c r="E178" s="191"/>
+      <c r="F178" s="191"/>
       <c r="G178" s="17"/>
       <c r="H178" s="17"/>
     </row>
@@ -5090,9 +5093,9 @@
       <c r="A179" s="17"/>
       <c r="B179" s="17"/>
       <c r="C179" s="17"/>
-      <c r="D179" s="140"/>
-      <c r="E179" s="140"/>
-      <c r="F179" s="140"/>
+      <c r="D179" s="191"/>
+      <c r="E179" s="191"/>
+      <c r="F179" s="191"/>
       <c r="G179" s="17"/>
       <c r="H179" s="17"/>
     </row>
@@ -5100,9 +5103,9 @@
       <c r="A180" s="17"/>
       <c r="B180" s="17"/>
       <c r="C180" s="17"/>
-      <c r="D180" s="140"/>
-      <c r="E180" s="140"/>
-      <c r="F180" s="140"/>
+      <c r="D180" s="191"/>
+      <c r="E180" s="191"/>
+      <c r="F180" s="191"/>
       <c r="G180" s="17"/>
       <c r="H180" s="17"/>
     </row>
@@ -5110,9 +5113,9 @@
       <c r="A181" s="17"/>
       <c r="B181" s="17"/>
       <c r="C181" s="17"/>
-      <c r="D181" s="140"/>
-      <c r="E181" s="140"/>
-      <c r="F181" s="140"/>
+      <c r="D181" s="191"/>
+      <c r="E181" s="191"/>
+      <c r="F181" s="191"/>
       <c r="G181" s="17"/>
       <c r="H181" s="17"/>
     </row>
@@ -5120,9 +5123,9 @@
       <c r="A182" s="17"/>
       <c r="B182" s="17"/>
       <c r="C182" s="17"/>
-      <c r="D182" s="140"/>
-      <c r="E182" s="140"/>
-      <c r="F182" s="140"/>
+      <c r="D182" s="191"/>
+      <c r="E182" s="191"/>
+      <c r="F182" s="191"/>
       <c r="G182" s="17"/>
       <c r="H182" s="17"/>
     </row>
@@ -5130,9 +5133,9 @@
       <c r="A183" s="17"/>
       <c r="B183" s="17"/>
       <c r="C183" s="17"/>
-      <c r="D183" s="140"/>
-      <c r="E183" s="140"/>
-      <c r="F183" s="140"/>
+      <c r="D183" s="191"/>
+      <c r="E183" s="191"/>
+      <c r="F183" s="191"/>
       <c r="G183" s="17"/>
       <c r="H183" s="17"/>
     </row>
@@ -5140,9 +5143,9 @@
       <c r="A184" s="17"/>
       <c r="B184" s="17"/>
       <c r="C184" s="17"/>
-      <c r="D184" s="140"/>
-      <c r="E184" s="140"/>
-      <c r="F184" s="140"/>
+      <c r="D184" s="191"/>
+      <c r="E184" s="191"/>
+      <c r="F184" s="191"/>
       <c r="G184" s="17"/>
       <c r="H184" s="17"/>
     </row>
@@ -5150,9 +5153,9 @@
       <c r="A185" s="17"/>
       <c r="B185" s="17"/>
       <c r="C185" s="17"/>
-      <c r="D185" s="140"/>
-      <c r="E185" s="140"/>
-      <c r="F185" s="140"/>
+      <c r="D185" s="191"/>
+      <c r="E185" s="191"/>
+      <c r="F185" s="191"/>
       <c r="G185" s="17"/>
       <c r="H185" s="17"/>
     </row>
@@ -5160,9 +5163,9 @@
       <c r="A186" s="17"/>
       <c r="B186" s="17"/>
       <c r="C186" s="17"/>
-      <c r="D186" s="140"/>
-      <c r="E186" s="140"/>
-      <c r="F186" s="140"/>
+      <c r="D186" s="191"/>
+      <c r="E186" s="191"/>
+      <c r="F186" s="191"/>
       <c r="G186" s="17"/>
       <c r="H186" s="17"/>
     </row>
@@ -5170,9 +5173,9 @@
       <c r="A187" s="17"/>
       <c r="B187" s="17"/>
       <c r="C187" s="17"/>
-      <c r="D187" s="140"/>
-      <c r="E187" s="140"/>
-      <c r="F187" s="140"/>
+      <c r="D187" s="191"/>
+      <c r="E187" s="191"/>
+      <c r="F187" s="191"/>
       <c r="G187" s="17"/>
       <c r="H187" s="17"/>
     </row>
@@ -5180,9 +5183,9 @@
       <c r="A188" s="17"/>
       <c r="B188" s="17"/>
       <c r="C188" s="17"/>
-      <c r="D188" s="140"/>
-      <c r="E188" s="140"/>
-      <c r="F188" s="140"/>
+      <c r="D188" s="191"/>
+      <c r="E188" s="191"/>
+      <c r="F188" s="191"/>
       <c r="G188" s="17"/>
       <c r="H188" s="17"/>
     </row>
@@ -5190,9 +5193,9 @@
       <c r="A189" s="17"/>
       <c r="B189" s="17"/>
       <c r="C189" s="17"/>
-      <c r="D189" s="140"/>
-      <c r="E189" s="140"/>
-      <c r="F189" s="140"/>
+      <c r="D189" s="191"/>
+      <c r="E189" s="191"/>
+      <c r="F189" s="191"/>
       <c r="G189" s="17"/>
       <c r="H189" s="17"/>
     </row>
@@ -5210,21 +5213,21 @@
       <c r="A191" s="44"/>
       <c r="B191" s="44"/>
       <c r="C191" s="44"/>
-      <c r="D191" s="142"/>
-      <c r="E191" s="142"/>
-      <c r="F191" s="142"/>
-      <c r="G191" s="142"/>
-      <c r="H191" s="142"/>
+      <c r="D191" s="188"/>
+      <c r="E191" s="188"/>
+      <c r="F191" s="188"/>
+      <c r="G191" s="188"/>
+      <c r="H191" s="188"/>
     </row>
     <row r="192" spans="1:8" ht="32.25" customHeight="1">
       <c r="A192" s="44"/>
       <c r="B192" s="44"/>
       <c r="C192" s="44"/>
-      <c r="D192" s="142"/>
-      <c r="E192" s="142"/>
-      <c r="F192" s="142"/>
-      <c r="G192" s="142"/>
-      <c r="H192" s="142"/>
+      <c r="D192" s="188"/>
+      <c r="E192" s="188"/>
+      <c r="F192" s="188"/>
+      <c r="G192" s="188"/>
+      <c r="H192" s="188"/>
     </row>
     <row r="193" spans="1:8">
       <c r="A193" s="17"/>
@@ -5260,108 +5263,88 @@
       <c r="A196" s="44"/>
       <c r="B196" s="44"/>
       <c r="C196" s="44"/>
-      <c r="D196" s="141"/>
-      <c r="E196" s="141"/>
-      <c r="F196" s="141"/>
-      <c r="G196" s="141"/>
-      <c r="H196" s="141"/>
+      <c r="D196" s="193"/>
+      <c r="E196" s="193"/>
+      <c r="F196" s="193"/>
+      <c r="G196" s="193"/>
+      <c r="H196" s="193"/>
     </row>
     <row r="197" spans="1:8" ht="17.25" customHeight="1">
       <c r="A197" s="44"/>
       <c r="B197" s="44"/>
       <c r="C197" s="44"/>
-      <c r="D197" s="141"/>
-      <c r="E197" s="141"/>
-      <c r="F197" s="141"/>
-      <c r="G197" s="141"/>
-      <c r="H197" s="141"/>
+      <c r="D197" s="193"/>
+      <c r="E197" s="193"/>
+      <c r="F197" s="193"/>
+      <c r="G197" s="193"/>
+      <c r="H197" s="193"/>
     </row>
     <row r="198" spans="1:8" ht="18" customHeight="1">
       <c r="A198" s="44"/>
       <c r="B198" s="44"/>
       <c r="C198" s="44"/>
-      <c r="D198" s="141"/>
-      <c r="E198" s="141"/>
-      <c r="F198" s="141"/>
-      <c r="G198" s="141"/>
-      <c r="H198" s="141"/>
+      <c r="D198" s="193"/>
+      <c r="E198" s="193"/>
+      <c r="F198" s="193"/>
+      <c r="G198" s="193"/>
+      <c r="H198" s="193"/>
     </row>
     <row r="199" spans="1:8">
       <c r="A199" s="44"/>
       <c r="B199" s="44"/>
       <c r="C199" s="44"/>
-      <c r="D199" s="141"/>
-      <c r="E199" s="141"/>
-      <c r="F199" s="141"/>
-      <c r="G199" s="141"/>
-      <c r="H199" s="141"/>
+      <c r="D199" s="193"/>
+      <c r="E199" s="193"/>
+      <c r="F199" s="193"/>
+      <c r="G199" s="193"/>
+      <c r="H199" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="132">
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="D58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="D47:H47"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D180:F180"/>
+    <mergeCell ref="D181:F181"/>
+    <mergeCell ref="D198:H198"/>
+    <mergeCell ref="D199:H199"/>
+    <mergeCell ref="D188:F188"/>
+    <mergeCell ref="D189:F189"/>
+    <mergeCell ref="D191:H191"/>
+    <mergeCell ref="D192:H192"/>
+    <mergeCell ref="D182:F182"/>
+    <mergeCell ref="D183:F183"/>
+    <mergeCell ref="D196:H196"/>
+    <mergeCell ref="D197:H197"/>
+    <mergeCell ref="D184:F184"/>
+    <mergeCell ref="D185:F185"/>
+    <mergeCell ref="D186:F186"/>
+    <mergeCell ref="D187:F187"/>
+    <mergeCell ref="F170:G170"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="D178:F178"/>
+    <mergeCell ref="D179:F179"/>
+    <mergeCell ref="F164:G164"/>
+    <mergeCell ref="F165:G165"/>
+    <mergeCell ref="F166:G166"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="F168:G168"/>
+    <mergeCell ref="F169:G169"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F161:G161"/>
+    <mergeCell ref="F162:G162"/>
+    <mergeCell ref="F163:G163"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="D145:H145"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F149:H149"/>
     <mergeCell ref="D76:F76"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="F26:H26"/>
@@ -5386,50 +5369,70 @@
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="D145:H145"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F161:G161"/>
-    <mergeCell ref="F162:G162"/>
-    <mergeCell ref="F163:G163"/>
-    <mergeCell ref="F170:G170"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="D178:F178"/>
-    <mergeCell ref="D179:F179"/>
-    <mergeCell ref="F164:G164"/>
-    <mergeCell ref="F165:G165"/>
-    <mergeCell ref="F166:G166"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="F168:G168"/>
-    <mergeCell ref="F169:G169"/>
-    <mergeCell ref="D180:F180"/>
-    <mergeCell ref="D181:F181"/>
-    <mergeCell ref="D198:H198"/>
-    <mergeCell ref="D199:H199"/>
-    <mergeCell ref="D188:F188"/>
-    <mergeCell ref="D189:F189"/>
-    <mergeCell ref="D191:H191"/>
-    <mergeCell ref="D192:H192"/>
-    <mergeCell ref="D182:F182"/>
-    <mergeCell ref="D183:F183"/>
-    <mergeCell ref="D196:H196"/>
-    <mergeCell ref="D197:H197"/>
-    <mergeCell ref="D184:F184"/>
-    <mergeCell ref="D185:F185"/>
-    <mergeCell ref="D186:F186"/>
-    <mergeCell ref="D187:F187"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="D58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="D47:H47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D84:E85">
@@ -5485,11 +5488,11 @@
       <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="B2" s="86"/>
-      <c r="C2" s="195" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="196"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="194" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="195"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
     </row>
@@ -5501,21 +5504,21 @@
       <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B4" s="87" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="197" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="198"/>
+      <c r="B4" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="196" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="197"/>
     </row>
     <row r="5" spans="1:10" s="63" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="234" t="s">
-        <v>176</v>
+      <c r="B5" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="198" t="s">
+        <v>171</v>
       </c>
       <c r="D5" s="199"/>
       <c r="E5" s="71"/>
@@ -5529,591 +5532,591 @@
       <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:10" s="64" customFormat="1" ht="38.25">
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="118" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="118" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="118" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="118" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="118" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="119" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="A8" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="106" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="113" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H8" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B9" s="107" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H9" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B10" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="101" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H10" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B11" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="101" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H11" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B12" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="102" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H12" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J12" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B13" s="107" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="101" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H13" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J13" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B14" s="107" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="101" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H14" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B15" s="107" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H15" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B16" s="106" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H16" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B17" s="107" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="101" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H17" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J17" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B18" s="107" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H18" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J18" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B19" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="101" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H19" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J19" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B20" s="106" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="103" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H20" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J20" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B21" s="107" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H21" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B22" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="103" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H22" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B23" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="101" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H23" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J23" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B24" s="107" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="114">
+        <v>42301</v>
+      </c>
+      <c r="H24" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1">
+      <c r="B25" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="104" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="119" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="119" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="119" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="119" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="119" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="119" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="120" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="A8" s="112" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="107" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="100" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="114" t="s">
+      <c r="E25" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="114" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="115">
+      <c r="F25" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="114">
         <v>42301</v>
       </c>
-      <c r="H8" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I8" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J8" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B9" s="108" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="101" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="114" t="s">
+      <c r="H25" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" s="116" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" s="125" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" s="111" customFormat="1" ht="45" customHeight="1" thickBot="1">
+      <c r="B26" s="108" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="120" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="121" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="115">
+      <c r="G26" s="122">
         <v>42301</v>
       </c>
-      <c r="H9" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J9" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B10" s="108" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="102" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H10" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I10" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J10" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B11" s="108" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="102" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H11" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J11" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B12" s="108" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="103" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H12" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I12" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J12" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B13" s="108" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="102" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H13" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I13" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J13" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B14" s="108" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="102" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H14" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I14" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J14" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B15" s="108" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H15" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I15" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J15" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B16" s="107" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="104" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H16" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I16" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J16" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B17" s="108" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="102" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H17" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I17" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J17" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B18" s="108" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="102" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H18" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I18" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B19" s="108" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="102" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H19" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I19" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J19" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B20" s="107" t="s">
-        <v>142</v>
-      </c>
-      <c r="C20" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="104" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H20" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I20" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J20" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B21" s="108" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="103" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H21" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I21" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J21" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B22" s="107" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="104" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H22" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I22" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J22" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B23" s="108" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="102" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H23" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I23" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J23" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B24" s="108" t="s">
+      <c r="H26" s="123" t="s">
+        <v>147</v>
+      </c>
+      <c r="I26" s="124" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="102" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H24" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I24" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J24" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1">
-      <c r="B25" s="108" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="105" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="115">
-        <v>42301</v>
-      </c>
-      <c r="H25" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="I25" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J25" s="126" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" s="112" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="B26" s="109" t="s">
+      <c r="J26" s="126" t="s">
         <v>148</v>
       </c>
-      <c r="C26" s="121" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="106" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="122" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="122" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="123">
-        <v>42301</v>
-      </c>
-      <c r="H26" s="124" t="s">
-        <v>150</v>
-      </c>
-      <c r="I26" s="125" t="s">
-        <v>149</v>
-      </c>
-      <c r="J26" s="127" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="27" spans="2:10">
-      <c r="H27" s="110"/>
-      <c r="I27" s="111"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6172,12 +6175,12 @@
       <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" ht="49.5" customHeight="1">
-      <c r="B2" s="88"/>
-      <c r="C2" s="195" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="194" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="203"/>
-      <c r="E2" s="196"/>
+      <c r="E2" s="195"/>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="60"/>
@@ -6186,8 +6189,8 @@
       <c r="E3" s="60"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
-      <c r="B4" s="89" t="s">
-        <v>160</v>
+      <c r="B4" s="88" t="s">
+        <v>155</v>
       </c>
       <c r="C4" s="202" t="str">
         <f>IF(NOT(ISBLANK('Requerimientos de Usuario'!C4)),'Requerimientos de Usuario'!C4," - ")</f>
@@ -6198,8 +6201,8 @@
     </row>
     <row r="5" spans="1:5" s="63" customFormat="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="89" t="s">
-        <v>84</v>
+      <c r="B5" s="88" t="s">
+        <v>83</v>
       </c>
       <c r="C5" s="202" t="str">
         <f>IF(NOT(ISBLANK('Requerimientos de Usuario'!C5)),'Requerimientos de Usuario'!C5," - ")</f>
@@ -6209,10 +6212,10 @@
       <c r="E5" s="202"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1">
       <c r="B7" s="206" t="s">
@@ -6231,10 +6234,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="201"/>
-      <c r="D8" s="92" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="91">
+      <c r="D8" s="91" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="90">
         <v>42287</v>
       </c>
     </row>
@@ -6361,34 +6364,34 @@
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="72" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="57" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="57" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="2:3">
@@ -6424,7 +6427,7 @@
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B31" sqref="B31:E31"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
@@ -6441,268 +6444,261 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" customFormat="1" ht="47.25" customHeight="1">
-      <c r="B2" s="96"/>
-      <c r="C2" s="208" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="210"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="226" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="228"/>
     </row>
     <row r="3" spans="2:6" ht="13.5" thickBot="1"/>
     <row r="4" spans="2:6" s="3" customFormat="1">
-      <c r="B4" s="211" t="s">
+      <c r="B4" s="229" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="212"/>
-      <c r="D4" s="128" t="s">
+      <c r="C4" s="230"/>
+      <c r="D4" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="E4" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="129" t="s">
+      <c r="F4" s="128" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="63.75">
-      <c r="B5" s="213" t="s">
+      <c r="B5" s="231" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="214"/>
-      <c r="D5" s="94" t="s">
+      <c r="C5" s="232"/>
+      <c r="D5" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="134" t="s">
+      <c r="E5" s="133" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="129"/>
+    </row>
+    <row r="6" spans="2:6" ht="25.5">
+      <c r="B6" s="231" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="232"/>
+      <c r="D6" s="92" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="129"/>
+    </row>
+    <row r="7" spans="2:6" ht="51">
+      <c r="B7" s="216" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="217"/>
+      <c r="D7" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="129"/>
+    </row>
+    <row r="8" spans="2:6" ht="178.5">
+      <c r="B8" s="216" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="217"/>
+      <c r="D8" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="129"/>
+    </row>
+    <row r="9" spans="2:6" ht="38.25">
+      <c r="B9" s="216" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="217"/>
+      <c r="D9" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="129"/>
+    </row>
+    <row r="10" spans="2:6" ht="25.5">
+      <c r="B10" s="216" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="217"/>
+      <c r="D10" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="134" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="129"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="218" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="219"/>
+      <c r="D11" s="211" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="130" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="25.5">
+      <c r="B12" s="222"/>
+      <c r="C12" s="223"/>
+      <c r="D12" s="233"/>
+      <c r="E12" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="130"/>
-    </row>
-    <row r="6" spans="2:6" ht="25.5">
-      <c r="B6" s="213" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="214"/>
-      <c r="D6" s="93" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" s="97" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="130"/>
-    </row>
-    <row r="7" spans="2:6" ht="51">
-      <c r="B7" s="217" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="218"/>
-      <c r="D7" s="93" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="135" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="204">
+      <c r="B13" s="216" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="217"/>
+      <c r="D13" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="130"/>
-    </row>
-    <row r="8" spans="2:6" ht="178.5">
-      <c r="B8" s="217" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="218"/>
-      <c r="D8" s="93" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="135" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="130"/>
-    </row>
-    <row r="9" spans="2:6" ht="38.25">
-      <c r="B9" s="217" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="218"/>
-      <c r="D9" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="135" t="s">
+      <c r="F13" s="129"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="218" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="219"/>
+      <c r="D14" s="211" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="131" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="220"/>
+      <c r="C15" s="221"/>
+      <c r="D15" s="212"/>
+      <c r="E15" s="96" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="131" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="220"/>
+      <c r="C16" s="221"/>
+      <c r="D16" s="214"/>
+      <c r="E16" s="96" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="130" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="25.5">
+      <c r="B17" s="220"/>
+      <c r="C17" s="221"/>
+      <c r="D17" s="214"/>
+      <c r="E17" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="131" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="25.5">
+      <c r="B18" s="222"/>
+      <c r="C18" s="223"/>
+      <c r="D18" s="215"/>
+      <c r="E18" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="131" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="89.25">
+      <c r="B19" s="216" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="217"/>
+      <c r="D19" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="130"/>
-    </row>
-    <row r="10" spans="2:6" ht="25.5">
-      <c r="B10" s="217" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="218"/>
-      <c r="D10" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="135" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="130"/>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="219" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="220"/>
-      <c r="D11" s="215" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="97" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="131" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="25.5">
-      <c r="B12" s="221"/>
-      <c r="C12" s="222"/>
-      <c r="D12" s="216"/>
-      <c r="E12" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="132" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="204">
-      <c r="B13" s="217" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="218"/>
-      <c r="D13" s="93" t="s">
-        <v>163</v>
-      </c>
-      <c r="E13" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="130"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="219" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="220"/>
-      <c r="D14" s="215" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="97" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="132" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="230"/>
-      <c r="C15" s="231"/>
-      <c r="D15" s="226"/>
-      <c r="E15" s="97" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="132" t="s">
+      <c r="F19" s="129"/>
+    </row>
+    <row r="20" spans="2:6" ht="12.75" customHeight="1">
+      <c r="B20" s="218" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="219"/>
+      <c r="D20" s="211" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" s="208"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="220"/>
+      <c r="C21" s="221"/>
+      <c r="D21" s="212"/>
+      <c r="E21" s="97" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="230"/>
-      <c r="C16" s="231"/>
-      <c r="D16" s="228"/>
-      <c r="E16" s="97" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="131" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="25.5">
-      <c r="B17" s="230"/>
-      <c r="C17" s="231"/>
-      <c r="D17" s="228"/>
-      <c r="E17" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="132" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="25.5">
-      <c r="B18" s="221"/>
-      <c r="C18" s="222"/>
-      <c r="D18" s="229"/>
-      <c r="E18" s="97" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="132" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="89.25">
-      <c r="B19" s="217" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="218"/>
-      <c r="D19" s="95" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="130"/>
-    </row>
-    <row r="20" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B20" s="219" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" s="220"/>
-      <c r="D20" s="215" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" s="97" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" s="223"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="230"/>
-      <c r="C21" s="231"/>
-      <c r="D21" s="226"/>
-      <c r="E21" s="98" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="224"/>
+      <c r="F21" s="209"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="230"/>
-      <c r="C22" s="231"/>
-      <c r="D22" s="226"/>
-      <c r="E22" s="97" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="224"/>
+      <c r="B22" s="220"/>
+      <c r="C22" s="221"/>
+      <c r="D22" s="212"/>
+      <c r="E22" s="96" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="209"/>
     </row>
     <row r="23" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B23" s="232"/>
-      <c r="C23" s="233"/>
-      <c r="D23" s="227"/>
-      <c r="E23" s="133" t="s">
-        <v>173</v>
-      </c>
-      <c r="F23" s="225"/>
+      <c r="B23" s="224"/>
+      <c r="C23" s="225"/>
+      <c r="D23" s="213"/>
+      <c r="E23" s="132" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C23"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
@@ -6713,6 +6709,13 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C12"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.67" right="0.75" top="0.79" bottom="0.7" header="0" footer="0.17"/>

</xml_diff>